<commit_message>
add basic export to doc (no image)
</commit_message>
<xml_diff>
--- a/gui/prompt_template.xlsx
+++ b/gui/prompt_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Toán" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
   <si>
     <t>Type</t>
   </si>
@@ -52,271 +52,110 @@
     <t>TL</t>
   </si>
   <si>
-    <t>Bạn là giáo viên Toán, hãy giúp tôi giải câu hỏi trắc nghiệm **{môn_học}** gồm 2 phần như sau:
-1. Nội dung câu hỏi:
+    <t xml:space="preserve">Cho nội dung và thực hiện tạo thêm cho tôi {copy_number} nội dung khác nhưng số liệu, đối tượng (nếu có) phải thay đổi. Các yêu cầu cụ thể như sau:
+Nội dung:
 {question}
-## Đáp án cho câu hỏi trên (nếu có): {correct_answer}
-2. Hình ảnh minh họa cho câu hỏi được cung cấp trong file ảnh đính kèm (nếu có).
-- Câu hỏi trong đề bài trên sẽ thuộc một trong các cấp độ nhận thức sau:
-* Cấp độ Nhận biết (NB): Học sinh nhớ các khái niệm cơ bản, có thể nêu lên hoặc nhận ra chúng khi được yêu cầu, các động từ thường dùng trong đặc tả và câu hỏi gồm: Kể, liệt kê, nêu tên, xác định, viết, tìm, nhận ra,...
-* Cấp độ Thông hiểu (TH): Học sinh hiểu các khái niệm cơ bản và có thể vận dụng chúng, khi chúng được thể hiện theo cách tương tự như cách giáo viên đã giảng hoặc như các ví dụ tiêu biểu về chúng trên lớp học, các động từ thường dùng trong đặc tả và câu hỏi: Giải thích, diễn giải, phác thảo, thảo luận, phân biệt, dự đoán, khẳng định lại, so sánh, mô tả..
-* Cấp độ Vận dụng (VD): Học sinh có thể hiểu được khái niệm ở một mức độ cao hơn “thông hiểu”, tạo ra được sự liên kết hợp lý giữa các khái niệm cơ bản và có thể vận dụng chúng để tổ chức lại các thông tin đã được trình bày giống với bài giảng của giáo viên hoặc trong sách giáo khoa. Các động từ thường dùng trong đặc tả và câu hỏi: Giải quyết, thể hiện, sử dụng, làm rõ, xây dựng, hoàn thiện, xem xét, làm sáng tỏ....
-* Cấp độ Vận dụng cao (VDC): Học sinh có thể sử dụng các kiến thức về môn học – chủ đề để giải quyết các vấn đề mới, không giống với những điều đã được học, hoặc trình bày trong sách giáo khoa, nhưng ở mức độ phù hợp nhiệm vụ, với kỹ năng và kiến thức được giảng dạy phù hợp với mức độ nhận thức này. Đây là những vấn đề, nhiệm vụ giống với các tình huống thực tiễn. Các động từ thường dùng trong đặc tả và câu hỏi: Tạo ra, phát hiện ra, soạn thảo, dự báo, lập kế hoạch, xây dựng, thiết kế, tưởng tượng, đề xuất, định hình.
-Kết quả trả về là dạng latex đối với các công thức toán học và công thức hóa học của các chất (các chỉ số cần được biểu diễn đúng định dạng) với các điều kiện:
-+ Sử dụng $...$ để bọc các công thức thay vì sử dụng \[...\] hay \(...\), không sử dụng \boxed{{}} trong công thức.
-- Trong phần **Lời giải** được chia thành 3 phần mỗi phần được phân cách bởi dấu và sẽ có cấu trúc như sau:
-+ Phần đầu sẽ là các số 1,2,3,4,.. sẽ tương đương với đáp án A,B,C,D,.. Ví dụ đáp án đúng là A thì sẽ là 1 (B đúng thì sẽ là 2,...)
-+ Phần hai sẽ là Đáp án đúng và **Gợi ý khi làm bài**
-+ Phần ba sẽ là Hướng dẫn giải chi tiết (Lời giải không quá 6 dòng)
-Lưu ý: - Trong phần **Lời giải**, các ký tự cần được giữ nguyên như trong ví dụ minh họa. Không sửa đổi hoặc lược bỏ bất kỳ dấu nào.
-- Câu hỏi phải được trình bày cấp độ nhận thức như sau:
-[NB]
-Câu 1: Nội dung câu hỏi
-Lời giải
-....
-[TH]
-Câu 2: Nội dung câu hỏi
-Lời giải
-- Tùy thuộc vào cấp độ nhận thức đầu ra cho các câu hỏi như sau:
-* Cấp độ Nhận biết [NB]: (lời giải tối thiểu 30 chữ ~ 2 dòng)
-Viết lại kiến thức. Kết luận viết lại khẳng định cho đáp án đúng.
-Nội dung trả về cần theo cấu trúc trong các ví dụ dưới, đừng thêm bất cứ gì khác, tôi sẽ chú thích trong dấu (...) giúp bạn hiểu rõ về từng phần nhưng đừng in ra trong kết quả trả về:
-```
-[NB]
-Câu 1: Cho khối chóp có chiều cao $h$ và diện tích đáy bằng $B$. Thể tích của khối chóp bằng
-A. $V = Bh$. 
-B. $V = \frac{{1}}{{9}}Bh$. 
-C. $V = 3Bh$. 
-D. $V = \frac{{1}}{{3}}Bh$. 
-Lời giải 
-4 (đáp án đúng, ở câu này là D - tương ứng với số 4)
-Đáp án đúng là D: (Tại đây là nội dung về phương pháp, gợi ý làm bài, hãy nhớ đưa ra phương pháp phù hợp)
-(Nội dung hướng dẫn giải chi tiết, bắt buộc có)
-Ta có công thức tính thể tích của khối chóp là: $V = \frac{{1}}{{3}}Bh$, trong đó B là diện tích đáy, h là chiều cao.
-(Hãy nhớ kết luận theo ý của đề bài và bắt buộc phải có)
-Vậy đáp án $V = \frac{{1}}{{3}}Bh$ là đáp án đúng.
-```
-* Cấp độ Thông hiểu (TH): Mức độ TH: (lời giải tối thiểu 45 chữ ~ 3 dòng)
-Lập luận, tính toán rõ ràng từng bước. Kết luận cần viết lại khẳng định cho đáp án đúng
-Nội dung trả về cần theo cấu trúc (tương tự ý trên) trong ví dụ sau:
-```
-[TH]
-Câu 1: Cho hàm số $f\left( x \right)$ liên tục trên $\mathbb{{R}}$. Gọi $F\left( x \right)$ là một nguyên hàm của hàm số $f\left( x \right)$ trên $\mathbb{{R}}$ thoả mãn $F\left( 2 \right) - F\left( 0 \right) = 10$. Khi đó $\int\limits_0^2 {{2f\left( x \right){{\text{{d}}}}x}} $ bằng
-A. $20$. 
-B. $5$. 
-C. $6$. 
-D. $4$. 
-Lời giải 
-1
-Đáp án đúng là A: (Tại đây là nội dung về phương pháp, gợi ý làm bài, hãy nhỡ đưa ra phương pháp giúp tôi)
-Ta có $\int\limits_0^2 {{f\left( x \right){{\text{{d}}}}x}} = \left. {{F\left( x \right)}} \right|_0^2 = F\left( 2 \right) - F\left( 0 \right) = 10$. 
-Suy ra $\int\limits_0^2 {{2f\left( x \right){{\text{{d}}}}x}} = 2\int\limits_0^2 {{f\left( x \right){{\text{{d}}}}x = 2.10 = }} 20$. 
-Vậy $\int\limits_0^2 {{2f\left( x \right){{\text{{d}}}}x}} = 20.$
-```
-* Cấp độ Vận dụng [VD] và Vận dụng cao [VDC]:
-Lập luận chặt chẽ từng bước để đưa ra kết luận; giải thích các cách tư duy hướng đến các đáp án sai (nếu có)
-Nội dung trả về cần theo cấu trúc (tương tự ý trên) trong ví dụ sau:
-```
-[VD]
-Câu 1: Cho hàm số $y = f(x) = a{{x^3}} + b{{x^2}} + cx + d{{\text{{ }}}}(a \ne 0)$ có đồ thị là đường cong được mô tả như sau: 
-- Hình dạng chung: Đồ thị có hình dạng chữ "N" lộn ngược, cho thấy hệ số của số hạng bậc ba là dương. 
-- Điểm cắt trục hoành (nghiệm): Đồ thị cắt trục hoành tại ba điểm phân biệt, nghĩa là hàm số có ba nghiệm thực phân biệt. Hai nghiệm dường như nằm đối xứng qua trục tung, gợi ý khả năng có một nghiệm tại x = 0 và hai nghiệm đối xứng nhau (ví dụ: x = -a và x = a). 
-- Điểm cắt trục tung: Đồ thị cắt trục tung tại gốc tọa độ (0,0), có nghĩa là f(0) = 0. Điều này xác nhận một trong ba nghiệm là x = 0. 
-- Cực trị: Đồ thị có một điểm cực đại địa phương (đỉnh cao nhất trong một vùng lân cận) và một điểm cực tiểu địa phương (đỉnh thấp nhất trong một vùng lân cận). 
-- Hành vi khi x tiến tới vô cùng: Khi x tiến tới dương vô cùng, f(x) cũng tiến tới dương vô cùng. Khi x tiến tới âm vô cùng, f(x) cũng tiến tới âm vô cùng. 
-- Tính liên tục và khả vi: Đồ thị là một đường cong mượt mà không có điểm gián đoạn hay góc nhọn, cho thấy hàm số liên tục và khả vi trên toàn bộ tập xác định của nó. 
-Số giá trị nguyên của tham số $m$ để phương trình $3f(x) - m = 0$ có 3 nghiệm phân biệt là:
-A. $10$. 
-B. $12$. 
-C. $13$. 
-D. $11$.
-Lời giải 
-4
-Đáp án đúng là D: (Tại đây là nội dung về phương pháp, gợi ý làm bài, hãy nhỡ đưa ra phương pháp giúp tôi)
-Ta có: $3f(x) - m = 0 \Leftrightarrow f(x) = \frac{{m}}{{3}}$. 
-Số nghiệm của phương trình trên là số giao điểm của đồ thị $y = f\left( x \right)$ và đường thẳng $y = \frac{{m}}{{3}}$ 
-Dựa vào đồ thị ta suy ra, phương trình $3f(x) - m = 0$có 3 nghiệm phân biệt khi và chỉ khi $ - 2 &lt; \frac{{m}}{{3}} &lt; 2 \Leftrightarrow - 6 &lt; m &lt; 6$.
-Vậy có 11 giá trị nguyên của tham số m thỏa mãn yêu cầu bài toán.
-```</t>
-  </si>
-  <si>
-    <t>Bạn là giáo viên Toán, giúp tôi giải chi tiết câu hỏi **Đúng sai** trong **{môn_học}** sau:
-1. Nội dung câu hỏi:
-{question}
-## Đáp án cho câu hỏi trên (nếu có) : {correct_answer}
-2. Hình ảnh minh họa cho câu hỏi được cung cấp trong file ảnh đính kèm (nếu có).
-3. Yêu cầu bắt buộc:
-- Câu hỏi trong đề bài trên sẽ thuộc một trong các cấp độ nhận thức sau:
-* Cấp độ Thông hiểu (TH): Học sinh hiểu các khái niệm cơ bản và có thể vận dụng chúng, khi chúng được thể hiện theo cách tương tự như cách giáo viên đã giảng hoặc như các ví dụ tiêu biểu về chúng trên lớp học, các động từ thường dùng trong đặc tả và câu hỏi: Giải thích, diễn giải, phác thảo, thảo luận, phân biệt, dự đoán, khẳng định lại, so sánh, mô tả..
-* Cấp độ Vận dụng (VD): Học sinh có thể hiểu được khái niệm ở một mức độ cao hơn “thông hiểu”, tạo ra được sự liên kết hợp lý giữa các khái niệm cơ bản và có thể vận dụng chúng để tổ chức lại các thông tin đã được trình bày giống với bài giảng của giáo viên hoặc trong sách giáo khoa. Các động từ thường dùng trong đặc tả và câu hỏi: Giải quyết, thể hiện, sử dụng, làm rõ, xây dựng, hoàn thiện, xem xét, làm sáng tỏ....
-- Kết quả trả về là dạng latex đối với các công thức toán học và công thức hóa học của các chất (các chỉ số cần được biểu diễn đúng định dạng) với các điều kiện:
-+ Sử dụng $...$ để bọc các công thức thay vì sử dụng \[...\] hay \(...\), không sử dụng \boxed{{}} trong công thức.
-- Trong phần **Lời giải** được chia thành 3 phần mỗi phần được phân cách bởi dấu và sẽ có cấu trúc như sau:
-+ Phần đầu sẽ là các số 1 và 0 tương ứng với đúng và sai. Ví dụ trong Câu 1 có a),b),c),d) nếu a) đúng thì sẽ là 1 b) sai sẽ là 0
-+ Phần hai sẽ là Đáp án đúng và **Gợi ý khi làm bài**
-+ Phần ba sẽ là Hướng dẫn giải chi tiết
-Lưu ý: - Trong phần **Lời giải**, các ký tự cần được giữ nguyên như trong ví dụ minh họa. Không sửa đổi hoặc lược bỏ bất kỳ dấu nào.
-- Nội dung trả về phải có đầy đủ cả câu hỏi và lời giải
-- Câu hỏi phải được trình bày cấp độ nhận thức như sau:
-[NB]
-Câu 1: Nội dung câu hỏi
-....
-[TH]
-Câu 2: Nội dung câu hỏi
-- Nội dung trả về cần theo đúng cấu trúc như sau:
-- Nội dung trả về cần theo cấu trúc trong ví dụ dưới, đừng thêm bất cứ gì khác, tôi sẽ chú thích trong dấu (...) giúp bạn hiểu rõ về từng phần nhưng đừng in ra trong kết quả trả về:
-```
-(cấp độ nhận thức, "" là kí tự xuống dòng trong Latex) [TH] 
-(Đề bài) Câu 1: Cho hàm số $y = \sqrt {{x + 1}} + \sqrt {{3 - x}}$.
-a) Giá trị nhỏ nhất của hàm số bằng $2$. 
-b) Giá trị lớn nhất của hàm số đạt được tại $x = - 1$. 
-c) Gọi $M,\,m$ lần lượt là giá trị lớn nhất và giá trị nhỏ nhất của hàm số. Khi đó $M + m = 4\sqrt 2 $. 
-d) Bất phương trình $\sqrt {{x + 1}} + \sqrt {{3 - x}} - 2m \geqslant 0,\forall x \in \left[ {{ - 1;3}} \right]$ ($m$ là tham số) khi $m \in \left( {{ - \infty ;2}} \right]$.
-Lời giải 
-1000 (lần lượt thể hiện đáp án đúng/sai, ở câu này là a-đúng, b-sai, c-sai, d-sai - tương ứng với 1000)
-Gợi ý làm bài:
-1. Xác định miền xác định của hàm số: Kiểm tra điều kiện để căn thức tồn tại, tìm khoảng giá trị của $x$.
-2. Tìm giá trị nhỏ nhất và lớn nhất: 
-- Tính đạo hàm để xét cực trị. 
-- Kiểm tra giá trị hàm số tại các điểm biên và điểm cực trị trong khoảng xác định.
-3. So sánh các đáp án: 
-- Kiểm tra xem giá trị lớn nhất và nhỏ nhất có đúng vị trí được nêu trong các đáp án không. 
-- Xem xét ý nghĩa của bất phương trình, liên hệ với giá trị nhỏ nhất của hàm số để suy luận khoảng tham số $m$.
-(Nội dung hướng dẫn giải chi tiết, bắt buộc có)
-Xét hàm số $y = \sqrt {{x + 1}} + \sqrt {{3 - x}}$ 
-Tập xác định $D = \left[ {{ - 1;3}} \right]$. 
-$y' = \frac{{1}}{{{{2\sqrt {{x + 1}} }}}} - \frac{{1}}{{{{2\sqrt {{3 - x}} }}}}$. 
-$y' = 0 \Leftrightarrow \frac{{1}}{{{{2\sqrt {{x + 1}} }}}} - \frac{{1}}{{{{2\sqrt {{3 - x}} }}}} = 0 \Leftrightarrow \sqrt {{x + 1}} = \sqrt {{3 - x}} \Leftrightarrow x = 1$.
-Bảng biến thiên
-**vẽ bảng biến thiên**
-(Hãy nhớ kết luận theo ý của đề bài theo thứ tự như sau “đề bài”-**đúng/sai**-giải thích, bắt buộc phải có kết luận)
-+) “Giá trị nhỏ nhất của hàm số bằng $2$” **đúng**. vì từ bảng biến thiên, suy ra $\mathop {{min}}\limits_{{\left[ {{ - 1;3}} \right]}} y = 2$ khi $x = - 1,x = 3$.
-+) “Giá trị lớn nhất của hàm số đạt được tại $x = - 1$” **sai**. vì từ bảng biến thiên, ta có: $\mathop {{max}}\limits_{{\left[ {{ - 1;3}} \right]}} y = 2\sqrt 2 $ khi $x = 1$.
-+) “Gọi $M,\,m$ lần lượt là giá trị lớn nhất và giá trị nhỏ nhất của hàm số. Khi đó $M + m = 4\sqrt 2 $” **sai**. Vì từ bảng biến thiên, ta có: $M + m = \mathop {{\max }}\limits_{{\left[ {{ - 1;3}} \right]}} y + \mathop {{\min }}\limits_{{\left[ {{ - 1;3}} \right]}} y = 2 + 2\sqrt 2 .$ 
-+) “Bất phương trình $\sqrt {{x + 1}} + \sqrt {{3 - x}} - 2m \geqslant 0,\forall x \in \left[ {{ - 1;3}} \right]$ ($m$ là tham số) khi $m \in \left( {{ - \infty ;2}} \right]$” **sai**. Ta có: $\sqrt {{x + 1}} + \sqrt {{3 - x}} - 2m \geqslant 0,\forall x \in \left[ {{ - 1;3}} \right]$ $\Leftrightarrow \sqrt {{x + 1}} + \sqrt {{3 - x}} \geqslant 2m,\forall x \in \left[ {{ - 1;3}} \right]$
-$\Leftrightarrow \mathop {{\min }}\limits_{{\left[ {{ - 1;3}} \right]}} \left( {{\sqrt {{x + 1}} + \sqrt {{3 - x}} }} \right) \geqslant 2m\;\left( 1 \right)$ suy ra $2m \leqslant 2 \Leftrightarrow m \leqslant 1$.
-```</t>
-  </si>
-  <si>
-    <t>Bạn là giáo viên Toán, giúp tôi giải chi tiết câu hỏi thuộc dạng điền đáp án đúng vào ô trống trong **{môn_học}** sau:
-1. Nội dung câu hỏi:
-{question}
-## Đáp án cho câu hỏi trên (nếu có) : {correct_answer}
-2. Hình ảnh minh họa cho câu hỏi được cung cấp trong file ảnh đính kèm (nếu có).
-3. Yêu cầu bắt buộc:
-- Câu hỏi trong đề bài trên sẽ thuộc một trong các cấp độ nhận thức sau:
-* Cấp độ Vận dụng (VD): Học sinh có thể hiểu được khái niệm ở một mức độ cao hơn “thông hiểu”, tạo ra được sự liên kết hợp lý giữa các khái niệm cơ bản và có thể vận dụng chúng để tổ chức lại các thông tin đã được trình bày giống với bài giảng của giáo viên hoặc trong sách giáo khoa. Các động từ thường dùng trong đặc tả và câu hỏi: Giải quyết, thể hiện, sử dụng, làm rõ, xây dựng, hoàn thiện, xem xét, làm sáng tỏ....
-* Cấp độ Vận dụng cao (VDC): Học sinh có thể sử dụng các kiến thức về môn học – chủ đề để giải quyết các vấn đề mới, không giống với những điều đã được học, hoặc trình bày trong sách giáo khoa, nhưng ở mức độ phù hợp nhiệm vụ, với kỹ năng và kiến thức được giảng dạy phù hợp với mức độ nhận thức này. Đây là những vấn đề, nhiệm vụ giống với các tình huống thực tiễn. Các động từ thường dùng trong đặc tả và câu hỏi: Tạo ra, phát hiện ra, soạn thảo, dự báo, lập kế hoạch, xây dựng, thiết kế, tưởng tượng, đề xuất, định hình.
-- Kết quả trả về là dạng latex đối với các công thức toán học và công thức hóa học của các chất (các chỉ số cần được biểu diễn đúng định dạng) với các điều kiện:
-+ Sử dụng $...$ để bọc các công thức thay vì sử dụng \[...\] hay \(...\), không sử dụng \boxed{{}} trong công thức.
-- Trong phần **Lời giải** được chia thành 3 phần mỗi phần được phân cách bởi dấu và sẽ có cấu trúc như sau:
-+ Phần đầu sẽ là [[Đáp án đúng]] (Lưu ý quan trọng: đáp án đúng cần phải được bao bọc bên trong của dấu [[Đáp án]])
-+ Phần hai sẽ là Đáp án đúng và **Gợi ý khi làm bài* (Đáp án đúng ở phần này sẽ không cần bao bọc trong dấu [[]])
-+ Phần ba sẽ là Hướng dẫn giải chi tiết
-Lưu ý: - Trong phần **Lời giải**, các ký tự cần được giữ nguyên như trong ví dụ minh họa. Không sửa đổi hoặc lược bỏ bất kỳ dấu nào.
-- Câu hỏi phải được trình bày cấp độ nhận thức như sau:
-[NB]
-Câu 1: Nội dung câu hỏi
-Lời giải
-....
-[TH]
-Câu 2: Nội dung câu hỏi
-Lời giải
-- Nội dung trả về cần theo cấu trúc trong ví dụ dưới, đừng thêm/thay đổi bất cứ thứ gì, tôi sẽ chú thích trong dấu (...) giúp bạn hiểu rõ về từng phần nhưng đừng in ra trong kết quả trả về:
-```
-[VD]
-Câu 1: Cho hàm số $y = f\left( x \right)$ có đạo hàm $f'\left( x \right) = \left( {{x - 8}} \right)\left( {{{{x^2}} - 9}} \right),\;\forall x \in \mathbb{{R}}$. Khi đó hàm số $g\left( x \right) = f\left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)$ có bao nhiêu điểm cực trị?
-Đáp án: [[3]].
-Lời giải
-1. Điều kiện để \( g(x) \) có cực trị: 
-Xét \( h'(x) = 0 \) hoặc \( f'(h(x)) = 0 \). 
-2. Tìm điểm đặc biệt của \( h(x) = \left|x^3 + 6x\right| + 5 \): 
-- Tìm nghiệm của \( x^3 + 6x = 0 \). 
-- Xét điều kiện \( \left|x^3 + 6x\right| + 5 = c \) với \( c \) là nghiệm làm \( f'(c) = 0 \).
-3. Tổng hợp các điểm cực trị của \( g(x) \): 
-Kiểm tra tất cả các trường hợp trên để tìm số điểm cực trị.
-(Nội dung hướng dẫn giải chi tiết, bắt buộc có)
-Ta có $g\left( x \right) = f\left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right) \Rightarrow g\prime \left( x \right) = {{\left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)^\prime }}.f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)$
-$ = \frac{{{{\left( {{{{x^3}} + 6x}} \right).\left( {{3{{x^2}} + 6}} \right)}}}}{{{{\left| {{{{x^3}} + 6x}} \right|}}}}.f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)$
-$ \Rightarrow g'\left( x \right) = 0 \Leftrightarrow \left[ \begin{{gathered}}
-x = 0 \hfill 
-f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right) = 0 \hfill 
-\end{{gathered}} \right.$.
-Có $f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right) = 0 \Leftrightarrow \left[ \begin{{gathered}}
-\left| {{{{x^3}} + 6x}} \right| + 5 = 8 \hfill 
-\left| {{{{x^3}} + 6x}} \right| + 5 = 3 \hfill 
-\left| {{{{x^3}} + 6x}} \right| + 5 = - 3 \hfill 
-\end{{gathered}} \right. \Leftrightarrow \left[ \begin{{gathered}}
-\left| {{{{x^3}} + 6x}} \right| = 3 \hfill 
-\left| {{{{x^3}} + 6x}} \right| = - 2 \hfill 
-\left| {{{{x^3}} + 6x}} \right| = - 8 \hfill 
-\end{{gathered}} \right. \Leftrightarrow \left| {{{{x^3}} + 6x}} \right| = 3\,\,\left( * \right)$ .
-Để xác định số nghiệm của $\left( * \right)$, ta có 2 cách sau:
-Cách 1: Áp dụng cho các bài toán có hàm phức tạp
-Xét hàm số $h\left( x \right) = {{x^3}} + 6x$, vì $h\prime \left( x \right) = 3{{x^2}} + 6 &gt; 0,\forall x \in \mathbb{{R}}$ nên $h\left( x \right)$ đồng biến trên $\mathbb{{R}}$. Ta có bảng biến thiên của hàm số $k\left( x \right) = \left| {{h\left( x \right)}} \right| = \left| {{{{x^3}} + 6x}} \right|$ như sau:
-***Tạo bảng xét dấu bằng mã latex***
-Cách 2: Phá dấu giá trị tuyệt đối và dùng máy tính cầm tay để giải 
-Khi đó $\left| {{{{x^3}} + 6x}} \right| = 3$ luôn có 2 nghiệm phân biệt.
-(Hãy nhớ kết luận theo ý của đề bài và bắt buộc phải có)
-Vậy $g'\left( x \right) = 0$ có 3 nghiệm phân biệt nên có hàm số $y = g\left( x \right)$ có 3 điểm cực trị. 
-```</t>
-  </si>
-  <si>
-    <t>Bạn là giáo viên Toán, giúp tôi giải chi tiết câu hỏi **Tự luận** **{môn_học}** gồm 2 phần như sau:
-1. Nội dung câu hỏi:
-{question}
-## Đáp án cho câu hỏi trên (nếu có) : {correct_answer}
-2. Hình ảnh minh họa cho câu hỏi được cung cấp trong file ảnh đính kèm (nếu có).
-- Câu hỏi trong đề bài trên sẽ thuộc một trong các cấp độ nhận thức sau:
-* Cấp độ Vận dụng (VD): Học sinh có thể hiểu được khái niệm ở một mức độ cao hơn “thông hiểu”, tạo ra được sự liên kết hợp lý giữa các khái niệm cơ bản và có thể vận dụng chúng để tổ chức lại các thông tin đã được trình bày giống với bài giảng của giáo viên hoặc trong sách giáo khoa. Các động từ thường dùng trong đặc tả và câu hỏi: Giải quyết, thể hiện, sử dụng, làm rõ, xây dựng, hoàn thiện, xem xét, làm sáng tỏ....
-* Cấp độ Vận dụng cao (VDC): Học sinh có thể sử dụng các kiến thức về môn học – chủ đề để giải quyết các vấn đề mới, không giống với những điều đã được học, hoặc trình bày trong sách giáo khoa, nhưng ở mức độ phù hợp nhiệm vụ, với kỹ năng và kiến thức được giảng dạy phù hợp với mức độ nhận thức này. Đây là những vấn đề, nhiệm vụ giống với các tình huống thực tiễn. Các động từ thường dùng trong đặc tả và câu hỏi: Tạo ra, phát hiện ra, soạn thảo, dự báo, lập kế hoạch, xây dựng, thiết kế, tưởng tượng, đề xuất, định hình.
-- Kết quả trả về là dạng latex đối với các công thức toán học và công thức hóa học của các chất (các chỉ số cần được biểu diễn đúng định dạng) với các điều kiện:
-+ Sử dụng $...$ để bọc các công thức thay vì sử dụng \[...\] hay \(...\), không sử dụng \boxed{{}} trong công thức.
-- Trong phần **Lời giải** được chia thành 2 phần mỗi phần được phân cách bởi dấu và sẽ có cấu trúc như sau:
-+ Phần đầu sẽ là Phương pháp giải và **Gợi ý khi làm bài* 
-+ Phần hai sẽ là Hướng dẫn giải chi tiết
-Lưu ý: - Trong phần **Lời giải**, các ký tự cần được giữ nguyên như trong ví dụ minh họa. Không sửa đổi hoặc lược bỏ bất kỳ dấu nào.
-- Câu hỏi phải được trình bày cấp độ nhận thức như sau:
-[NB]
-Câu 1: Nội dung câu hỏi
-Lời giải
-....
-[TH]
-Câu 2: Nội dung câu hỏi
-Lời giải
-- Nội dung trả về cần theo đúng cấu trúc như sau:
-```
-[VD]
-Câu 1: Cho hàm số $y = f\left( x \right)$ có đạo hàm $f'\left( x \right) = \left( {{x - 8}} \right)\left( {{{{x^2}} - 9}} \right),\;\forall x \in \mathbb{{R}}$. Khi đó hàm số $g\left( x \right) = f\left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)$ có bao nhiêu điểm cực trị?
-Lời giải
-1. Xét \( u = |x^3 + 6x| + 5 \), tìm các khoảng thay đổi của \( u \) dựa trên nghiệm của \( x^3 + 6x = 0 \). 
-2. Phân tích hàm \( g(x) \) dựa trên \( g'(x) = f'(u) \cdot u'(x) \). 
-3. Xác định các giá trị của \( u \) tại đó \( f'(u) = 0 \). 
-4. Kiểm tra số nghiệm của \( g'(x) = 0 \) trên từng khoảng.
-Ta có $g\left( x \right) = f\left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right) \Rightarrow g\prime \left( x \right) = {{\left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)^\prime }}.f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)$
-$ = \frac{{{{\left( {{{{x^3}} + 6x}} \right).\left( {{3{{x^2}} + 6}} \right)}}}}{{{{\left| {{{{x^3}} + 6x}} \right|}}}}.f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right)$
-$ \Rightarrow g'\left( x \right) = 0 \Leftrightarrow \left[ \begin{{gathered}}
-x = 0 \hfill \\
-f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right) = 0 \hfill \\ 
-\end{{gathered}} \right.$.
-Có $f\prime \left( {{\left| {{{{x^3}} + 6x}} \right| + 5}} \right) = 0 \Leftrightarrow \left[ \begin{{gathered}}
-\left| {{{{x^3}} + 6x}} \right| + 5 = 8 \hfill \\
-\left| {{{{x^3}} + 6x}} \right| + 5 = 3 \hfill \\
-\left| {{{{x^3}} + 6x}} \right| + 5 = - 3 \hfill \\ 
-\end{{gathered}} \right. \Leftrightarrow \left[ \begin{{gathered}}
-\left| {{{{x^3}} + 6x}} \right| = 3 \hfill \\
-\left| {{{{x^3}} + 6x}} \right| = - 2 \hfill \\
-\left| {{{{x^3}} + 6x}} \right| = - 8 \hfill \\ 
-\end{{gathered}} \right. \Leftrightarrow \left| {{{{x^3}} + 6x}} \right| = 3\,\,\left( * \right)$ .
-Để xác định số nghiệm của $\left( * \right)$, ta có 2 cách sau:
-Cách 1: Áp dụng cho các bài toán có hàm phức tạp
-Xét hàm số $h\left( x \right) = {{x^3}} + 6x$, vì $h\prime \left( x \right) = 3{{x^2}} + 6 &gt; 0,\forall x \in \mathbb{{R}}$ nên $h\left( x \right)$ đồng biến trên $\mathbb{{R}}$. Ta có bảng biến thiên của hàm số $k\left( x \right) = \left| {{h\left( x \right)}} \right| = \left| {{{{x^3}} + 6x}} \right|$ như sau:
-***Tạo bảng xét dấu bằng mã latex***
-Cách 2: Phá dấu giá trị tuyệt đối và dùng máy tính cầm tay để giải 
-Khi đó $\left| {{{{x^3}} + 6x}} \right| = 3$ luôn có 2 nghiệm phân biệt.
-Vậy $g'\left( x \right) = 0$ có 3 nghiệm phân biệt nên có hàm số $y = g\left( x \right)$ có 3 điểm cực trị. 
-Đáp án: 3.
-```</t>
+Lời giải:
+{correct_answer}
+Yêu cầu:
+- Ở phần nội dung câu hỏi, bám sát nội dung, đừng thêm hay bớt gì. Độ khó tương đương với câu gốc. Với nội dung câu hỏi trắc nghiệm thì là dạng **trắc nghiệm 1 đáp án đúng**
+- Ở phần nội dung lời giải, hãy bám sát vào lời giải trong nội dung trên, đừng thêm hay bớt gì nhưng bạn có thể tùy biến như đảo đáp án.
+- Các công thức tính phải được chuyển về mã Latex và bọc trong dấu $...$, **đảm bảo các ký tự backslash \ trong mã Latex được thoát đúng cách trong JSON (\\), nhưng giữ nguyên không đổi kí tự xuống dòng (\n)**.
+- Kết quả chỉ trả về nội dung tạo thêm ở dạng JSON (theo mẫu ví dụ dưới)
+    + Số câu ở nội dung là số nào thì trường "questionNumber" tương ứng với số đó (Ví dụ: ở nội dung là "Câu 2: đề bài...", thì "questionNumber": 2, ở nội dung là "Câu 3: đề bài...", thì "questionNumber": 3)
+    + Ở trường "list" là mảng chứa thông tin của **tất cả {copy_number} nội dung** được tạo thêm.
+    + Trường "tables" là dữ liệu bảng (nếu có).
+- Đừng thêm bất cứ thông tin nào khác.
+Mẫu ví dụ 1 dưới dạng JSON, đừng thêm chú thích trong () khi trả về kết quả:
+{
+    "questionNumber": (số câu tương ứng trong nội dung),
+    "list": [
+        {
+            "content": "Có 5 quyển sách toán và 2 quyển sách văn trên một giá sách. Hỏi có bao nhiêu cách lấy ra một quyển sách từ giá sách đó?",
+            "image": null,
+            "tables": null (nếu có bảng hãy thêm tại đây),
+            "options": [
+                "A. $7$.",
+                "B. $10$.",
+                "C. $5$.",
+                "D. $2$."
+            ],
+            "guide": "Chọn A.\nĐể lấy ra một quyển sách từ giá sách, ta có thể lấy một quyển sách toán hoặc một quyển sách văn.\nCó 5 quyển sách toán, nên có 5 cách để lấy ra một quyển sách toán.\nCó 2 quyển sách văn, nên có 2 cách để lấy ra một quyển sách văn.\nVậy, số cách lấy ra một quyển sách là 5 + 2 = 7.",
+            "answer": "A"
+        },
+        {
+            "content": "Trong một giỏ trái cây có 6 quả cam và 3 quả táo. Hỏi có bao nhiêu cách chọn ra một quả từ giỏ trái cây đó?",
+            "image": null,
+            "tables": null (nếu có bảng hãy thêm tại đây),
+            "options": [
+                "A. $18$.",
+                "B. $9$.",
+                "C. $6$.",
+                "D. $3$."
+            ],
+            "guide": "Chọn B.\nĐể chọn ra một quả từ giỏ trái cây, ta có thể chọn một quả cam hoặc một quả táo.\nCó 6 quả cam, nên có 6 cách để chọn ra một quả cam.\nCó 3 quả táo, nên có 3 cách để chọn ra một quả táo.\nVậy, số cách chọn ra một quả là 6 + 3 = 9.",
+            "answer": "B"
+        },
+        ...
+    ]
+}
+Mẫu ví dụ 2 dưới dạng JSON, đừng thêm chú thích trong () khi trả về kết quả:
+{
+    "questionNumber": (số câu tương ứng trong nội dung),
+    "list": [
+        {
+            "content": "Một hộp chứa 18 viên bi gồm 3 viên bi đỏ, 6 viên bi xanh và 9 viên bi vàng.",
+            "image": null,
+            "tables": null (nếu có bảng hãy thêm tại đây),
+            "options": [
+                "a) Số cách chọn được 1 viên bi từ hộp là 18.",
+                "b) Số cách chọn 3 viên bi đủ 3 màu là 3.",
+                "c) Số cách chọn ra 4 viên bi trong đó có 1 viên bi đỏ, 2 viên bi xanh và 1 viên bi vàng là 405.",
+                "d) Số cách chọn ra 4 viên bi lấy được đủ 3 màu là 1268."
+            ],
+            "guide": "a) Đúng\nChọn 1 viên bi từ hộp chứa 18 viên bi ta có 18 cách.\n\nb) Sai\nChọn 3 viên bi gồm 1 viên bi đỏ, 1 viên bi xanh và 1 viên bi vàng có: $C_3^1.C_6^1.C_9^1 = 162$ (cách)\n\nc) Đúng\nChọn từ hộp 4 viên bi trong đó có 1 viên bi đỏ, 2 viên bi xanh và 1 viên bi vàng có:\n$C_3^1.C_6^2.C_9^1 = 3.15.9 = 405$ (cách)\n\nd) Sai\nChọn 4 viên bi từ 18 viên bi có: $C_{18}^4 = 3060$ (cách).\nXét trường hợp chọn 4 viên bi không đủ 3 màu:\n+ Chọn 4 viên bi chỉ gồm màu đỏ và màu xanh có: $C_3^1.C_6^3 + C_3^3.C_6^1 + C_3^2.C_6^2 = 111$.\n+ Chọn 4 viên bi chỉ gồm màu xanh và màu vàng có: $C_6^1.C_9^3 + C_6^3.C_9^1 + C_6^2.C_9^2 = 1224$.\n+ Chọn 4 viên bi chỉ gồm màu đỏ và màu vàng có: $C_3^1.C_9^3 + C_3^3.C_9^1 + C_3^2.C_9^2 = 369$.\n+ Chọn 4 viên bi chỉ gồm màu xanh có: $C_6^4 = 15$\n+ Chọn 4 viên bi chỉ gồm màu vàng có: $C_9^4 = 126$\nVậy số cách chọn 4 viên bi từ 18 viên bi mà 4 viên bi đó đủ ba màu là: $3060 - 111 - 1224 - 369 - 15 - 126 = 1215$ (cách).",
+            "answer": "a) Đúng, b) Sai, c) Đúng, d) Sai"
+        },
+        {
+            "content": "Một túi có 20 viên kẹo, trong đó có 5 viên kẹo dâu, 8 viên kẹo cam và 7 viên kẹo chanh.",
+            "image": null,
+            "tables": null (nếu có bảng hãy thêm tại đây),
+            "options": [
+                "a) Số cách chọn được 1 viên kẹo từ túi là 20.",
+                "b) Số cách chọn ra 4 viên kẹo trong đó có 1 viên kẹo dâu, 2 viên kẹo cam và 1 viên kẹo chanh là 280.",
+                "c) Số cách chọn 3 viên kẹo đủ 3 vị là 280.",
+                "d) Số cách chọn ra 4 viên kẹo lấy được đủ 3 vị là 965."
+            ],
+            "guide": "a) Đúng\nChọn 1 viên kẹo từ túi chứa 20 viên kẹo ta có 20 cách.\nb) Đúng\nChọn từ túi 4 viên kẹo trong đó có 1 viên kẹo dâu, 2 viên kẹo cam và 1 viên kẹo chanh có:\n$C_5^1.C_8^2.C_7^1 = 5.28.7 = 980$ (cách)\nc) Sai\nChọn 3 viên kẹo gồm 1 viên kẹo dâu, 1 viên kẹo cam và 1 viên kẹo chanh có: $C_5^1.C_8^1.C_7^1 = 280$ (cách)\nd) Sai\nChọn 4 viên kẹo từ 20 viên kẹo có: $C_{20}^4 = 4845$ (cách).\nXét trường hợp chọn 4 viên kẹo không đủ 3 vị:\n+ Chọn 4 viên kẹo chỉ gồm vị dâu và vị cam có: $C_5^1.C_8^3 + C_5^3.C_8^1 + C_5^2.C_8^2 = 500$.\n+ Chọn 4 viên kẹo chỉ gồm vị cam và vị chanh có: $C_8^1.C_7^3 + C_8^3.C_7^1 + C_8^2.C_7^2 = 1078$.\n+ Chọn 4 viên kẹo chỉ gồm vị dâu và vị chanh có: $C_5^1.C_7^3 + C_5^3.C_7^1 + C_5^2.C_7^2 = 475$.\n+ Chọn 4 viên kẹo chỉ gồm vị cam có: $C_8^4 = 70$\n+ Chọn 4 viên kẹo chỉ gồm vị chanh có: $C_7^4 = 35$\nVậy số cách chọn 4 viên kẹo từ 20 viên kẹo mà 4 viên kẹo đó đủ ba vị là: $4845 - 500 - 1078 - 475 - 70 - 35 = 2687$ (cách).",
+            "answer": "a) Đúng, b) Đúng, c) Sai, d) Sai"
+        },
+        ...
+    ]
+}
+Mẫu ví dụ 3 dưới dạng JSON, đừng thêm chú thích trong () khi trả về kết quả:
+{
+    "questionNumber": (số câu tương ứng trong nội dung),
+    "list": [
+        {
+            "content": "Một người có 7 chiếc áo khác nhau trong đó có 4 chiếc áo trắng; có 5 chiếc cà vạt khác nhau trong đó có 3 chiếc cà vạt màu vàng. Có bao nhiêu cách chọn 1 chiếc áo và 1 chiếc cà vạt sao cho đã chọn áo trắng thì không chọn cà vạt màu vàng?",
+            "image": null,
+            "tables": null (nếu có bảng hãy thêm tại đây),
+            "options": [],
+            "guide": "TH1:\nChọn 1 áo trắng có 4 cách\nChọn 1 cà vạt không phải màu vàng có 2 cách.\nDo đó có $4.2 = 8$ cách chọn 1 áo trắng và 1 cà vạt không phải màu vàng.\nTH2: \nChọn 1 áo không phải màu trắng có 3 cách.\nChọn 1 cà vạt bất kì có 5 cách.\nDo đó có: $3.5 = 15$ cách chọn 1 áo không phải màu trắng và 1 cà vạt bất kì.\nTheo quy tắc cộng ta có: $8 + 15 = 23$ cách chọn thỏa mãn yêu cầu bài toán.",
+            "answer": 23
+        },
+        {
+        "content": "Một người có 6 đôi giày khác nhau trong đó có 2 đôi giày thể thao; có 4 chiếc mũ khác nhau trong đó có 1 chiếc mũ lưỡi trai. Có bao nhiêu cách chọn 1 đôi giày và 1 chiếc mũ sao cho đã chọn giày thể thao thì không chọn mũ lưỡi trai?",
+            "image": null,
+            "tables": null (nếu có bảng hãy thêm tại đây),
+            "options": [],
+            "guide": "TH1:\nChọn 1 đôi giày thể thao có 2 cách\nChọn 1 mũ không phải lưỡi trai có 3 cách.\nDo đó có $2.3 = 6$ cách chọn 1 đôi giày thể thao và 1 mũ không phải lưỡi trai.\nTH2:\nChọn 1 đôi giày không phải giày thể thao có 4 cách.\nChọn 1 mũ bất kì có 4 cách.\nDo đó có: $4.4 = 16$ cách chọn 1 đôi giày không phải giày thể thao và 1 mũ bất kì.\nTheo quy tắc cộng ta có: $6 + 16 = 22$ cách chọn thỏa mãn yêu cầu bài toán.",
+            "answer": "22"
+        },
+    ...
+    ]
+}
+</t>
   </si>
 </sst>
 </file>
@@ -367,16 +206,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -663,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,7 +522,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -695,7 +531,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="64.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -703,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -711,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>